<commit_message>
Update Index.xlsx: Modified content to reflect latest changes
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\program\VSCode\md\AN_Collections\GithubStorage\ch32_application_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB066D87-C3FF-4C44-A071-DFDDA7A950F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C3A7B5-B3F7-4E52-A290-11EC4F13780C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{B3C2C8E5-E98A-4560-9C89-70683FDDB0B4}"/>
   </bookViews>
@@ -217,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +228,15 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -251,12 +260,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -272,9 +284,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -313,7 +329,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F20C98E0-EC21-4FA5-95A7-F381479833AC}" name="表3" displayName="表3" ref="A1:G2" totalsRowShown="0">
   <autoFilter ref="A1:G2" xr:uid="{F20C98E0-EC21-4FA5-95A7-F381479833AC}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FCBBF4A2-03CB-4883-8E68-90DEB846908D}" name="文件" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{FCBBF4A2-03CB-4883-8E68-90DEB846908D}" name="文件" dataDxfId="5" dataCellStyle="超链接"/>
     <tableColumn id="8" xr3:uid="{2B89B17F-3453-47BF-A4C3-7D99CD563975}" name="标题" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{EDB8B225-1A54-4245-85C0-DC125B05E45D}" name="类型" dataDxfId="3">
       <calculatedColumnFormula>IFERROR(VLOOKUP(INT(MID($A2,FIND("AN",$A2)+2,2)),Index[],2,FALSE),"")</calculatedColumnFormula>
@@ -658,7 +674,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -694,7 +710,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -716,9 +732,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C6CAF562-2619-45FE-9264-34AA75AF1797}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Add application note AN22000 for CH32H417 SDMMC interface
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\program\VSCode\md\AN_Collections\dist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\program\VSCode\md\AN_Collections\GithubStorage\ch32_application_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306869BC-E2F3-4EB3-B4DF-063ECCAB3B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91598056-D1C8-4FF8-8BFE-DCA2109BA654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{B3C2C8E5-E98A-4560-9C89-70683FDDB0B4}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="类型Index" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">文件列表!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">文件列表!$A$1:$F$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -222,6 +222,17 @@
   </si>
   <si>
     <t>--</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AN22000.pdf</t>
+  </si>
+  <si>
+    <t>本应用笔记详细介绍了如何使用沁恒微电子（WCH）的高性能RISC-V微控制器CH32H417的高速SDMMC 接口，来驱动嵌入式多媒体卡（eMMC）和从模式通信。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SDMMC多媒体卡和从模式通信</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -280,7 +291,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -305,18 +316,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -336,6 +344,12 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -350,21 +364,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F20C98E0-EC21-4FA5-95A7-F381479833AC}" name="表3" displayName="表3" ref="A1:I2" totalsRowShown="0">
-  <autoFilter ref="A1:I2" xr:uid="{F20C98E0-EC21-4FA5-95A7-F381479833AC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F20C98E0-EC21-4FA5-95A7-F381479833AC}" name="表3" displayName="表3" ref="A1:I3" totalsRowShown="0">
+  <autoFilter ref="A1:I3" xr:uid="{F20C98E0-EC21-4FA5-95A7-F381479833AC}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{FCBBF4A2-03CB-4883-8E68-90DEB846908D}" name="文件" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{915FD8AC-706D-4E1C-A85F-1735C0A4E667}" name="链接CH" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{915FD8AC-706D-4E1C-A85F-1735C0A4E667}" name="链接CH" dataDxfId="6">
       <calculatedColumnFormula>HYPERLINK("https://github.com/openwch/ch32_application_notes/blob/main/zh/"&amp;表3[[#This Row],[文件]],"Link")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A29C0DDC-6656-4A87-9641-B46EAFE59C8A}" name="链接EN" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{2B89B17F-3453-47BF-A4C3-7D99CD563975}" name="标题" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{EDB8B225-1A54-4245-85C0-DC125B05E45D}" name="类型" dataDxfId="5">
+    <tableColumn id="9" xr3:uid="{A29C0DDC-6656-4A87-9641-B46EAFE59C8A}" name="链接EN" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{2B89B17F-3453-47BF-A4C3-7D99CD563975}" name="标题" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{EDB8B225-1A54-4245-85C0-DC125B05E45D}" name="类型" dataDxfId="3">
       <calculatedColumnFormula>IFERROR(VLOOKUP(INT(MID($A2,FIND("AN",$A2)+2,2)),Index[],2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{49F37FEB-3215-4B10-8D00-0B74E36C8895}" name="发布日期" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{51B42D66-90E9-41C1-A474-37DD2DBDE15D}" name="更新日期" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{05417962-2E32-4EE8-A769-CB6582724555}" name="说明" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{49F37FEB-3215-4B10-8D00-0B74E36C8895}" name="发布日期" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{51B42D66-90E9-41C1-A474-37DD2DBDE15D}" name="更新日期" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{05417962-2E32-4EE8-A769-CB6582724555}" name="说明" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{0A3FAFAC-1BAE-4E66-AD5E-6E0216D8CD05}" name="备注"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -702,14 +716,14 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.77734375" customWidth="1"/>
     <col min="8" max="8" width="46.77734375" bestFit="1" customWidth="1"/>
@@ -770,6 +784,34 @@
       </c>
       <c r="H2" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <f>HYPERLINK("https://github.com/openwch/ch32_application_notes/blob/main/zh/"&amp;表3[[#This Row],[文件]],"Link")</f>
+        <v>Link</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="8" t="str">
+        <f>IFERROR(VLOOKUP(INT(MID($A3,FIND("AN",$A3)+2,2)),Index[],2,FALSE),"")</f>
+        <v>SDMMC</v>
+      </c>
+      <c r="F3" s="3">
+        <v>45915</v>
+      </c>
+      <c r="G3" s="3">
+        <v>45916</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Index.xlsx add link to Gitee source
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\program\VSCode\md\AN_Collections\GithubStorage\ch32_application_notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91598056-D1C8-4FF8-8BFE-DCA2109BA654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5537003F-EB12-4337-812C-3E4221FBD089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{B3C2C8E5-E98A-4560-9C89-70683FDDB0B4}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="类型Index" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">文件列表!$A$1:$F$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">文件列表!$A$1:$H$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -233,6 +233,14 @@
   </si>
   <si>
     <t>SDMMC多媒体卡和从模式通信</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CH Gitee镜像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EN Gitee镜像</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -291,21 +299,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -316,17 +318,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="13">
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -339,7 +358,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -364,22 +383,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F20C98E0-EC21-4FA5-95A7-F381479833AC}" name="表3" displayName="表3" ref="A1:I3" totalsRowShown="0">
-  <autoFilter ref="A1:I3" xr:uid="{F20C98E0-EC21-4FA5-95A7-F381479833AC}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FCBBF4A2-03CB-4883-8E68-90DEB846908D}" name="文件" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{915FD8AC-706D-4E1C-A85F-1735C0A4E667}" name="链接CH" dataDxfId="6">
-      <calculatedColumnFormula>HYPERLINK("https://github.com/openwch/ch32_application_notes/blob/main/zh/"&amp;表3[[#This Row],[文件]],"Link")</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F20C98E0-EC21-4FA5-95A7-F381479833AC}" name="文件索引表" displayName="文件索引表" ref="A1:K3" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:K3" xr:uid="{F20C98E0-EC21-4FA5-95A7-F381479833AC}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{FCBBF4A2-03CB-4883-8E68-90DEB846908D}" name="文件" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{915FD8AC-706D-4E1C-A85F-1735C0A4E667}" name="链接CH" dataDxfId="1">
+      <calculatedColumnFormula>HYPERLINK("https://github.com/openwch/ch32_application_notes/blob/main/zh/"&amp;文件索引表[[#This Row],[文件]],"Github")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A29C0DDC-6656-4A87-9641-B46EAFE59C8A}" name="链接EN" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{2B89B17F-3453-47BF-A4C3-7D99CD563975}" name="标题" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{EDB8B225-1A54-4245-85C0-DC125B05E45D}" name="类型" dataDxfId="3">
+    <tableColumn id="10" xr3:uid="{C1CA5325-BEFE-4310-8DC2-EB0EDF1E6B79}" name="CH Gitee镜像" dataDxfId="0" dataCellStyle="超链接">
+      <calculatedColumnFormula>HYPERLINK("https://gitee.com/SYT_23/ch32_application_notes/raw/main/zh/"&amp;文件索引表[[#This Row],[文件]],"Gitee")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{A29C0DDC-6656-4A87-9641-B46EAFE59C8A}" name="链接EN" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{5E4BA809-651A-4796-B06B-3034F6BA9AE9}" name="EN Gitee镜像" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{2B89B17F-3453-47BF-A4C3-7D99CD563975}" name="标题" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{EDB8B225-1A54-4245-85C0-DC125B05E45D}" name="类型" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(VLOOKUP(INT(MID($A2,FIND("AN",$A2)+2,2)),Index[],2,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{49F37FEB-3215-4B10-8D00-0B74E36C8895}" name="发布日期" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{51B42D66-90E9-41C1-A474-37DD2DBDE15D}" name="更新日期" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{05417962-2E32-4EE8-A769-CB6582724555}" name="说明" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{0A3FAFAC-1BAE-4E66-AD5E-6E0216D8CD05}" name="备注"/>
+    <tableColumn id="3" xr3:uid="{49F37FEB-3215-4B10-8D00-0B74E36C8895}" name="发布日期" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{51B42D66-90E9-41C1-A474-37DD2DBDE15D}" name="更新日期" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{05417962-2E32-4EE8-A769-CB6582724555}" name="说明" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{0A3FAFAC-1BAE-4E66-AD5E-6E0216D8CD05}" name="备注" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -713,109 +736,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F8D6A9-DB12-4BB0-8144-B232BE534B97}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" customWidth="1"/>
-    <col min="8" max="8" width="46.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="str">
-        <f>HYPERLINK("https://github.com/openwch/ch32_application_notes/blob/main/zh/"&amp;表3[[#This Row],[文件]],"Link")</f>
-        <v>Link</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="3" t="str">
+        <f>HYPERLINK("https://github.com/openwch/ch32_application_notes/blob/main/zh/"&amp;文件索引表[[#This Row],[文件]],"Github")</f>
+        <v>Github</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f>HYPERLINK("https://gitee.com/SYT_23/ch32_application_notes/raw/main/zh/"&amp;文件索引表[[#This Row],[文件]],"Gitee")</f>
+        <v>Gitee</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="2" t="str">
+      <c r="G2" s="1" t="str">
         <f>IFERROR(VLOOKUP(INT(MID($A2,FIND("AN",$A2)+2,2)),Index[],2,FALSE),"")</f>
         <v>PWR</v>
       </c>
-      <c r="F2" s="3">
+      <c r="H2" s="2">
         <v>45910</v>
       </c>
-      <c r="G2" s="3">
+      <c r="I2" s="2">
         <v>45910</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="5" t="str">
-        <f>HYPERLINK("https://github.com/openwch/ch32_application_notes/blob/main/zh/"&amp;表3[[#This Row],[文件]],"Link")</f>
-        <v>Link</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="3" t="str">
+        <f>HYPERLINK("https://github.com/openwch/ch32_application_notes/blob/main/zh/"&amp;文件索引表[[#This Row],[文件]],"Github")</f>
+        <v>Github</v>
+      </c>
+      <c r="C3" s="3" t="str">
+        <f>HYPERLINK("https://gitee.com/SYT_23/ch32_application_notes/raw/main/zh/"&amp;文件索引表[[#This Row],[文件]],"Gitee")</f>
+        <v>Gitee</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="8" t="str">
+      <c r="G3" s="1" t="str">
         <f>IFERROR(VLOOKUP(INT(MID($A3,FIND("AN",$A3)+2,2)),Index[],2,FALSE),"")</f>
         <v>SDMMC</v>
       </c>
-      <c r="F3" s="3">
+      <c r="H3" s="2">
         <v>45915</v>
       </c>
-      <c r="G3" s="3">
+      <c r="I3" s="2">
         <v>45916</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="6"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>